<commit_message>
Azure Url Crawl in CSV
</commit_message>
<xml_diff>
--- a/Azure URLS.xlsx
+++ b/Azure URLS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\PycharmProjects\AzureApi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B8DD9EE-E948-4542-B044-2FA590D1C284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B576C3-5FDD-4DE1-AEBA-52740475E48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E2C2CB8-884E-4D53-A5C7-A3F42B40EBA7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>A family</t>
   </si>
@@ -348,6 +348,60 @@
   </si>
   <si>
     <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/gpu-accelerated/ndmi300xv5-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/gpu-accelerated/nvv3-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/gpu-accelerated/nvv4-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/gpu-accelerated/nvadsa10v5-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/gpu-accelerated/nvadsv710-v5-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/fpga-accelerated/np-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/fpga-accelerated/nm-ads-ma35d-series?tabs=Basics</t>
+  </si>
+  <si>
+    <t>HB</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/high-performance-compute/hb-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/high-performance-compute/hbv2-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/high-performance-compute/hbv3-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/high-performance-compute/hbv4-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/high-performance-compute/hc-family</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/high-performance-compute/hc-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/high-performance-compute/hx-series?tabs=sizebasic</t>
   </si>
 </sst>
 </file>
@@ -411,10 +465,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -734,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C336CB-1B74-45AD-B5F6-831708C20714}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,6 +1289,91 @@
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>113</v>
+      </c>
+      <c r="B100" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>118</v>
+      </c>
+      <c r="B104" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
database element sorted by instance name
</commit_message>
<xml_diff>
--- a/Azure URLS.xlsx
+++ b/Azure URLS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\PycharmProjects\AzureApi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixwissel/PycharmProjects/AzureApi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B576C3-5FDD-4DE1-AEBA-52740475E48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7852128B-4299-6A44-9B40-449802258229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E2C2CB8-884E-4D53-A5C7-A3F42B40EBA7}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{2E2C2CB8-884E-4D53-A5C7-A3F42B40EBA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t>A family</t>
   </si>
   <si>
-    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/general-purpose/a-family</t>
-  </si>
-  <si>
-    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/general-purpose/b-family</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -194,9 +188,6 @@
     <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/compute-optimized/fxmdsv2-series?tabs=sizebasic</t>
   </si>
   <si>
-    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/compute-optimized/fx-series?tabs=sizebasic</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -402,6 +393,18 @@
   </si>
   <si>
     <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/high-performance-compute/hx-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/general-purpose/av2-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/general-purpose/bsv2-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/general-purpose/basv2-series?tabs=sizebasic</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/de-de/azure/virtual-machines/sizes/general-purpose/bpsv2-series?tabs=sizebasic</t>
   </si>
 </sst>
 </file>
@@ -784,604 +787,609 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C336CB-1B74-45AD-B5F6-831708C20714}">
-  <dimension ref="A1:B106"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="209" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="B35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>45</v>
       </c>
-      <c r="B42" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="B50" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>53</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="B70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="B71" t="s">
         <v>74</v>
       </c>
-      <c r="B69" t="s">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
         <v>76</v>
       </c>
-      <c r="B70" t="s">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+      <c r="B74" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
         <v>80</v>
       </c>
-      <c r="B73" t="s">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+      <c r="B80" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>87</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B82" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
         <v>90</v>
       </c>
-      <c r="B81" t="s">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+      <c r="B88" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
         <v>97</v>
       </c>
-      <c r="B87" t="s">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+      <c r="B94" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="1" t="s">
+      <c r="B95" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
         <v>104</v>
       </c>
-      <c r="B93" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
         <v>105</v>
       </c>
-      <c r="B94" t="s">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
+      <c r="B99" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>110</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B101" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
         <v>113</v>
       </c>
-      <c r="B100" t="s">
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
+      <c r="B105" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
         <v>118</v>
-      </c>
-      <c r="B104" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" xr:uid="{260AF3C9-223F-4573-BE3C-0629A35FEE43}"/>
-    <hyperlink ref="B48" r:id="rId2" xr:uid="{C698BF1F-2E4A-4EBA-AB0E-1EE379BD30C2}"/>
-    <hyperlink ref="B54" r:id="rId3" xr:uid="{2F49304E-D61C-44C4-B90F-CDB8B2E3B979}"/>
-    <hyperlink ref="B92" r:id="rId4" xr:uid="{E90C082C-9368-42C4-95B6-91B1DE35E371}"/>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{260AF3C9-223F-4573-BE3C-0629A35FEE43}"/>
+    <hyperlink ref="B55" r:id="rId2" xr:uid="{2F49304E-D61C-44C4-B90F-CDB8B2E3B979}"/>
+    <hyperlink ref="B93" r:id="rId3" xr:uid="{E90C082C-9368-42C4-95B6-91B1DE35E371}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{CBEDAB3E-FD1F-854F-A175-9080C075BFE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>